<commit_message>
Script now functions without upper or lower limit to ISO ppm
</commit_message>
<xml_diff>
--- a/csatest.xlsx
+++ b/csatest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matlab\Clean Pantheon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matlab\development_pantheon_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77839FA9-E9CA-4693-917E-E889FCFC469E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8481A21E-A197-4633-BCFF-E1EA4416C39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="6345" windowWidth="22725" windowHeight="11640" xr2:uid="{688D2840-3B0A-4492-88A9-75D2C6293E50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{688D2840-3B0A-4492-88A9-75D2C6293E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -125,7 +125,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -231,7 +231,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -373,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,14 +384,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.01</v>
+        <v>-1.02</v>
       </c>
       <c r="B1">
         <v>25</v>
@@ -413,7 +413,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>15.05</v>
       </c>
       <c r="B3">
         <v>17</v>

</xml_diff>

<commit_message>
Updated read me, minor updates to other scripts such as correcting the directory
</commit_message>
<xml_diff>
--- a/csatest.xlsx
+++ b/csatest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matlab\development_pantheon_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8481A21E-A197-4633-BCFF-E1EA4416C39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A465E93A-A8AF-4AE6-81EF-63A498F8DBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{688D2840-3B0A-4492-88A9-75D2C6293E50}"/>
   </bookViews>
@@ -384,14 +384,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-1.02</v>
+        <v>0.01</v>
       </c>
       <c r="B1">
         <v>25</v>

</xml_diff>